<commit_message>
code modification to remove BaseStep
</commit_message>
<xml_diff>
--- a/DataSheet/RegistrationData.xlsx
+++ b/DataSheet/RegistrationData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prade\eclipse-workspace\CapstoneProject\DataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prade\git\CapstoneProject\CapstoneProject\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8330AD61-AA88-42F3-A336-DACF578880AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A868F474-FECD-4671-B1D3-C028662ACC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
testing the maven test
</commit_message>
<xml_diff>
--- a/DataSheet/RegistrationData.xlsx
+++ b/DataSheet/RegistrationData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="33">
   <si>
     <t>FirstName</t>
   </si>
@@ -143,6 +143,9 @@
     <t>Last name is required.
 Address is required.
 Username is required.</t>
+  </si>
+  <si>
+    <t>This username already exists.</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
         <v>21</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>